<commit_message>
issue #142 - modif héritage cardinalité title cfd2d678166b6c98774a2c808afcf2e5ed8cd7a1
</commit_message>
<xml_diff>
--- a/ig/issue142-correctif-slices-sdo-task/StructureDefinition-sdo-document-reference.xlsx
+++ b/ig/issue142-correctif-slices-sdo-task/StructureDefinition-sdo-document-reference.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="495">
   <si>
     <t>Property</t>
   </si>
@@ -1099,6 +1099,211 @@
   </si>
   <si>
     <t>DocumentEntry.mimeType, DocumentEntry.languageCode, DocumentEntry.URI, DocumentEntry.size, DocumentEntry.hash, DocumentEntry.title, DocumentEntry.creationTime</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.id</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.extension</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.contentType</t>
+  </si>
+  <si>
+    <t>Mime type of the content, with charset etc.</t>
+  </si>
+  <si>
+    <t>Identifies the type of the data in the attachment and allows a method to be chosen to interpret or render the data. Includes mime type parameters such as charset where appropriate.</t>
+  </si>
+  <si>
+    <t>Note that FHIR strings SHALL NOT exceed 1MB in size</t>
+  </si>
+  <si>
+    <t>Processors of the data need to be able to know how to interpret the data.</t>
+  </si>
+  <si>
+    <t>text/plain; charset=UTF-8, image/png</t>
+  </si>
+  <si>
+    <t>The mime type of an attachment. Any valid mime type is allowed.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/mimetypes|4.0.1</t>
+  </si>
+  <si>
+    <t>Attachment.contentType</t>
+  </si>
+  <si>
+    <t>./mediaType, ./charset</t>
+  </si>
+  <si>
+    <t>ED.2+ED.3/RP.2+RP.3. Note conversion may be needed if old style values are being used</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.language</t>
+  </si>
+  <si>
+    <t>Human language of the content (BCP-47)</t>
+  </si>
+  <si>
+    <t>The human language of the content. The value can be any valid value according to BCP 47.</t>
+  </si>
+  <si>
+    <t>Users need to be able to choose between the languages in a set of attachments.</t>
+  </si>
+  <si>
+    <t>en-AU</t>
+  </si>
+  <si>
+    <t>Attachment.language</t>
+  </si>
+  <si>
+    <t>./language</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base64Binary
+</t>
+  </si>
+  <si>
+    <t>Data inline, base64ed</t>
+  </si>
+  <si>
+    <t>The actual data of the attachment - a sequence of bytes, base64 encoded.</t>
+  </si>
+  <si>
+    <t>The base64-encoded data SHALL be expressed in the same character set as the base resource XML or JSON.</t>
+  </si>
+  <si>
+    <t>The data needs to able to be transmitted inline.</t>
+  </si>
+  <si>
+    <t>Attachment.data</t>
+  </si>
+  <si>
+    <t>./data</t>
+  </si>
+  <si>
+    <t>ED.5</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url
+</t>
+  </si>
+  <si>
+    <t>Uri where the data can be found</t>
+  </si>
+  <si>
+    <t>A location where the data can be accessed.</t>
+  </si>
+  <si>
+    <t>If both data and url are provided, the url SHALL point to the same content as the data contains. Urls may be relative references or may reference transient locations such as a wrapping envelope using cid: though this has ramifications for using signatures. Relative URLs are interpreted relative to the service url, like a resource reference, rather than relative to the resource itself. If a URL is provided, it SHALL resolve to actual data.</t>
+  </si>
+  <si>
+    <t>The data needs to be transmitted by reference.</t>
+  </si>
+  <si>
+    <t>http://www.acme.com/logo-small.png</t>
+  </si>
+  <si>
+    <t>Attachment.url</t>
+  </si>
+  <si>
+    <t>./reference/literal</t>
+  </si>
+  <si>
+    <t>RP.1+RP.2 - if they refer to a URL (see v2.6)</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unsignedInt
+</t>
+  </si>
+  <si>
+    <t>Number of bytes of content (if url provided)</t>
+  </si>
+  <si>
+    <t>The number of bytes of data that make up this attachment (before base64 encoding, if that is done).</t>
+  </si>
+  <si>
+    <t>The number of bytes is redundant if the data is provided as a base64binary, but is useful if the data is provided as a url reference.</t>
+  </si>
+  <si>
+    <t>Representing the size allows applications to determine whether they should fetch the content automatically in advance, or refuse to fetch it at all.</t>
+  </si>
+  <si>
+    <t>Attachment.size</t>
+  </si>
+  <si>
+    <t>N/A (needs data type R3 proposal)</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.hash</t>
+  </si>
+  <si>
+    <t>Hash of the data (sha-1, base64ed)</t>
+  </si>
+  <si>
+    <t>The calculated hash of the data using SHA-1. Represented using base64.</t>
+  </si>
+  <si>
+    <t>The hash is calculated on the data prior to base64 encoding, if the data is based64 encoded. The hash is not intended to support digital signatures. Where protection against malicious threats a digital signature should be considered, see [Provenance.signature](provenance-definitions.html#Provenance.signature) for mechanism to protect a resource with a digital signature.</t>
+  </si>
+  <si>
+    <t>Included so that applications can verify that the contents of a location have not changed due to technical failures (e.g., storage rot, transport glitch, incorrect version).</t>
+  </si>
+  <si>
+    <t>Attachment.hash</t>
+  </si>
+  <si>
+    <t>.integrityCheck[parent::ED/integrityCheckAlgorithm="SHA-1"]</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.title</t>
+  </si>
+  <si>
+    <t>Label to display in place of the data</t>
+  </si>
+  <si>
+    <t>A label or set of text to display in place of the data.</t>
+  </si>
+  <si>
+    <t>Applications need a label to display to a human user in place of the actual data if the data cannot be rendered or perceived by the viewer.</t>
+  </si>
+  <si>
+    <t>Official Corporate Logo</t>
+  </si>
+  <si>
+    <t>Attachment.title</t>
+  </si>
+  <si>
+    <t>./title/data</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
+</t>
+  </si>
+  <si>
+    <t>Date attachment was first created</t>
+  </si>
+  <si>
+    <t>The date that the attachment was first created.</t>
+  </si>
+  <si>
+    <t>This is often tracked as an integrity issue for use of the attachment.</t>
+  </si>
+  <si>
+    <t>Attachment.creation</t>
   </si>
   <si>
     <t>DocumentReference.content.format</t>
@@ -1649,7 +1854,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AQ46"/>
+  <dimension ref="A1:AQ56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1658,8 +1863,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="46.23828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="46.23828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="50.828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="50.828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
@@ -1677,7 +1882,7 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="35.69140625" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
@@ -5919,20 +6124,18 @@
         <v>79</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>350</v>
+        <v>282</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>351</v>
+        <v>283</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>353</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>79</v>
@@ -5957,13 +6160,13 @@
         <v>79</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>354</v>
+        <v>79</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>355</v>
+        <v>79</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>79</v>
@@ -5981,7 +6184,7 @@
         <v>79</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>349</v>
+        <v>285</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>80</v>
@@ -5990,50 +6193,50 @@
         <v>92</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>356</v>
+        <v>79</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>335</v>
+        <v>113</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>357</v>
+        <v>79</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP35" t="s" s="2">
-        <v>358</v>
+        <v>79</v>
       </c>
       <c r="AQ35" t="s" s="2">
-        <v>359</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>79</v>
@@ -6042,19 +6245,19 @@
         <v>79</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>274</v>
+        <v>140</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>361</v>
+        <v>141</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>362</v>
+        <v>287</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>363</v>
+        <v>143</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -6092,31 +6295,31 @@
         <v>79</v>
       </c>
       <c r="AB36" t="s" s="2">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="AC36" t="s" s="2">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="AD36" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>360</v>
+        <v>288</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>79</v>
@@ -6125,7 +6328,7 @@
         <v>79</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>364</v>
+        <v>106</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>79</v>
@@ -6142,10 +6345,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6165,19 +6368,23 @@
         <v>79</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>282</v>
+        <v>115</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>283</v>
+        <v>352</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="O37" t="s" s="2">
+        <v>355</v>
+      </c>
       <c r="P37" t="s" s="2">
         <v>79</v>
       </c>
@@ -6189,7 +6396,7 @@
         <v>79</v>
       </c>
       <c r="T37" t="s" s="2">
-        <v>79</v>
+        <v>356</v>
       </c>
       <c r="U37" t="s" s="2">
         <v>79</v>
@@ -6201,13 +6408,13 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>79</v>
+        <v>357</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>79</v>
+        <v>358</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>79</v>
@@ -6225,7 +6432,7 @@
         <v>79</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>285</v>
+        <v>359</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>80</v>
@@ -6234,10 +6441,10 @@
         <v>92</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>79</v>
@@ -6246,7 +6453,7 @@
         <v>79</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>113</v>
+        <v>360</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>79</v>
@@ -6255,7 +6462,7 @@
         <v>79</v>
       </c>
       <c r="AP37" t="s" s="2">
-        <v>79</v>
+        <v>361</v>
       </c>
       <c r="AQ37" t="s" s="2">
         <v>79</v>
@@ -6263,21 +6470,21 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>79</v>
@@ -6286,21 +6493,23 @@
         <v>79</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>141</v>
+        <v>363</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>287</v>
+        <v>364</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="O38" s="2"/>
+        <v>354</v>
+      </c>
+      <c r="O38" t="s" s="2">
+        <v>365</v>
+      </c>
       <c r="P38" t="s" s="2">
         <v>79</v>
       </c>
@@ -6312,7 +6521,7 @@
         <v>79</v>
       </c>
       <c r="T38" t="s" s="2">
-        <v>79</v>
+        <v>366</v>
       </c>
       <c r="U38" t="s" s="2">
         <v>79</v>
@@ -6324,43 +6533,43 @@
         <v>79</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AB38" t="s" s="2">
-        <v>144</v>
+        <v>79</v>
       </c>
       <c r="AC38" t="s" s="2">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="AD38" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>146</v>
+        <v>79</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>288</v>
+        <v>367</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>79</v>
@@ -6369,7 +6578,7 @@
         <v>79</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>106</v>
+        <v>368</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>79</v>
@@ -6386,45 +6595,45 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>290</v>
+        <v>79</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>79</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>140</v>
+        <v>370</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>291</v>
+        <v>371</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>292</v>
+        <v>372</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>143</v>
+        <v>373</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>152</v>
+        <v>374</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>79</v>
@@ -6473,19 +6682,19 @@
         <v>79</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>293</v>
+        <v>375</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>79</v>
@@ -6494,7 +6703,7 @@
         <v>79</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>106</v>
+        <v>376</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>79</v>
@@ -6503,7 +6712,7 @@
         <v>79</v>
       </c>
       <c r="AP39" t="s" s="2">
-        <v>79</v>
+        <v>377</v>
       </c>
       <c r="AQ39" t="s" s="2">
         <v>79</v>
@@ -6511,10 +6720,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6525,7 +6734,7 @@
         <v>80</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>79</v>
@@ -6534,21 +6743,23 @@
         <v>79</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="O40" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>383</v>
+      </c>
       <c r="P40" t="s" s="2">
         <v>79</v>
       </c>
@@ -6560,7 +6771,7 @@
         <v>79</v>
       </c>
       <c r="T40" t="s" s="2">
-        <v>79</v>
+        <v>384</v>
       </c>
       <c r="U40" t="s" s="2">
         <v>79</v>
@@ -6596,37 +6807,37 @@
         <v>79</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>368</v>
+        <v>385</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>226</v>
+        <v>105</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>372</v>
+        <v>79</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>373</v>
+        <v>79</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>375</v>
+        <v>79</v>
       </c>
       <c r="AP40" t="s" s="2">
-        <v>79</v>
+        <v>387</v>
       </c>
       <c r="AQ40" t="s" s="2">
         <v>79</v>
@@ -6634,10 +6845,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6648,7 +6859,7 @@
         <v>80</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>79</v>
@@ -6657,21 +6868,23 @@
         <v>79</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>195</v>
+        <v>389</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="O41" s="2"/>
+        <v>392</v>
+      </c>
+      <c r="O41" t="s" s="2">
+        <v>393</v>
+      </c>
       <c r="P41" t="s" s="2">
         <v>79</v>
       </c>
@@ -6695,13 +6908,13 @@
         <v>79</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>213</v>
+        <v>79</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>380</v>
+        <v>79</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>381</v>
+        <v>79</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>79</v>
@@ -6719,13 +6932,13 @@
         <v>79</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>376</v>
+        <v>394</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>104</v>
@@ -6737,10 +6950,10 @@
         <v>79</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>382</v>
+        <v>79</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>79</v>
@@ -6749,18 +6962,18 @@
         <v>79</v>
       </c>
       <c r="AP41" t="s" s="2">
-        <v>219</v>
+        <v>79</v>
       </c>
       <c r="AQ41" t="s" s="2">
-        <v>384</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6783,18 +6996,20 @@
         <v>93</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="O42" s="2"/>
+        <v>399</v>
+      </c>
+      <c r="O42" t="s" s="2">
+        <v>400</v>
+      </c>
       <c r="P42" t="s" s="2">
         <v>79</v>
       </c>
@@ -6842,7 +7057,7 @@
         <v>79</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>385</v>
+        <v>401</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>80</v>
@@ -6854,36 +7069,36 @@
         <v>104</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>390</v>
+        <v>105</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>391</v>
+        <v>79</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>393</v>
+        <v>79</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP42" t="s" s="2">
-        <v>394</v>
+        <v>79</v>
       </c>
       <c r="AQ42" t="s" s="2">
-        <v>395</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6891,7 +7106,7 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>92</v>
@@ -6903,21 +7118,23 @@
         <v>79</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>195</v>
+        <v>282</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="O43" s="2"/>
+        <v>354</v>
+      </c>
+      <c r="O43" t="s" s="2">
+        <v>406</v>
+      </c>
       <c r="P43" t="s" s="2">
         <v>79</v>
       </c>
@@ -6929,7 +7146,7 @@
         <v>79</v>
       </c>
       <c r="T43" t="s" s="2">
-        <v>79</v>
+        <v>407</v>
       </c>
       <c r="U43" t="s" s="2">
         <v>79</v>
@@ -6941,13 +7158,13 @@
         <v>79</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>213</v>
+        <v>79</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>400</v>
+        <v>79</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>401</v>
+        <v>79</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>79</v>
@@ -6965,7 +7182,7 @@
         <v>79</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>80</v>
@@ -6983,30 +7200,30 @@
         <v>79</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>402</v>
+        <v>79</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>404</v>
+        <v>79</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP43" t="s" s="2">
-        <v>219</v>
+        <v>79</v>
       </c>
       <c r="AQ43" t="s" s="2">
-        <v>405</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7026,22 +7243,20 @@
         <v>79</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>195</v>
+        <v>411</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>409</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>79</v>
@@ -7066,13 +7281,13 @@
         <v>79</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>213</v>
+        <v>79</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>411</v>
+        <v>79</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>412</v>
+        <v>79</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>79</v>
@@ -7090,7 +7305,7 @@
         <v>79</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>80</v>
@@ -7108,30 +7323,30 @@
         <v>79</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>402</v>
+        <v>79</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>402</v>
+        <v>79</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP44" t="s" s="2">
-        <v>219</v>
+        <v>79</v>
       </c>
       <c r="AQ44" t="s" s="2">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7151,19 +7366,19 @@
         <v>79</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>225</v>
+        <v>420</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7189,13 +7404,13 @@
         <v>79</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>79</v>
+        <v>421</v>
       </c>
       <c r="Z45" t="s" s="2">
-        <v>79</v>
+        <v>422</v>
       </c>
       <c r="AA45" t="s" s="2">
         <v>79</v>
@@ -7213,7 +7428,7 @@
         <v>79</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>80</v>
@@ -7225,36 +7440,36 @@
         <v>104</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>226</v>
+        <v>105</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>228</v>
+        <v>423</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>229</v>
+        <v>335</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>230</v>
+        <v>424</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AP45" t="s" s="2">
-        <v>79</v>
+        <v>425</v>
       </c>
       <c r="AQ45" t="s" s="2">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7265,7 +7480,7 @@
         <v>80</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>79</v>
@@ -7274,19 +7489,19 @@
         <v>79</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>420</v>
+        <v>274</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7336,40 +7551,1272 @@
         <v>79</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ46" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="AN46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ46" t="s" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G47" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q47" s="2"/>
+      <c r="R47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP47" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ47" t="s" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G48" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q48" s="2"/>
+      <c r="R48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP48" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ48" t="s" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G49" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="O49" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="P49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q49" s="2"/>
+      <c r="R49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AM49" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ49" t="s" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q50" s="2"/>
+      <c r="R50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK46" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AL46" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="AO46" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AP46" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AQ46" t="s" s="2">
-        <v>427</v>
+      <c r="AK50" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO50" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="AP50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ50" t="s" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G51" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="O51" s="2"/>
+      <c r="P51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q51" s="2"/>
+      <c r="R51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP51" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AQ51" t="s" s="2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP52" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="AQ52" t="s" s="2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="O53" s="2"/>
+      <c r="P53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q53" s="2"/>
+      <c r="R53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AO53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP53" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AQ53" t="s" s="2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="P54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q54" s="2"/>
+      <c r="R54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="AO54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP54" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AQ54" t="s" s="2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="O55" s="2"/>
+      <c r="P55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q55" s="2"/>
+      <c r="R55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AO55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP55" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ55" t="s" s="2">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Q56" s="2"/>
+      <c r="R56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="AO56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AP56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AQ56" t="s" s="2">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>